<commit_message>
0529    FilterDefinitions.jsfl 框架补充 sprintf-js 更名
</commit_message>
<xml_diff>
--- a/计划更新.xlsx
+++ b/计划更新.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="F:\04_ps\沙雕动画\_素材库\WindowSWF-master\WindowSWF-master\AnJsflScript\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{3EAA3280-5C62-4908-A026-C4BD760B437E}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E650493-BEFB-45AE-9D44-512FDE26E417}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-60" yWindow="-60" windowWidth="25720" windowHeight="13800" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView minimized="1" xWindow="1470" yWindow="1950" windowWidth="19200" windowHeight="9980" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="长期目标" sheetId="1" r:id="rId1"/>
@@ -871,7 +871,7 @@
   <dimension ref="B2:E16"/>
   <sheetViews>
     <sheetView zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>
@@ -974,7 +974,7 @@
   <dimension ref="A2:L9"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="175" zoomScaleNormal="175" workbookViewId="0">
-      <selection activeCell="B4" sqref="B4"/>
+      <selection activeCell="C6" sqref="C6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14"/>

</xml_diff>